<commit_message>
MATCHES 10 AND 20
</commit_message>
<xml_diff>
--- a/scoresheets/MATCH10.xlsx
+++ b/scoresheets/MATCH10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab4ea91dc20bd738/Documents/college/freshman/spring/coaching/DUOACHATT/scoresheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab4ea91dc20bd738/Documents/GitHub/DUOACHCATT-5-15-21-STATS/scoresheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_62F1D62F365428EBBDF08FAB6C17C44C6D0DAA31" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{42C3BF0B-C96A-4398-B6BF-69C6E03978D6}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="11_62F1D62F365428EBBDF08FAB6C17C44C6D0DAA31" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CC0F4CD9-5370-4341-8A52-DCC296A80661}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -863,18 +863,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -883,33 +910,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -944,16 +944,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:E34"/>
+    <sheetView topLeftCell="B6" zoomScale="105" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1283,17 +1283,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="s">
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="55"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="73"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -1330,7 +1330,7 @@
       <c r="N2" s="53"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="74" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1341,10 +1341,12 @@
       <c r="E3" s="3"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="58"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1356,19 +1358,21 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="59"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10">
+        <v>2</v>
+      </c>
       <c r="G5" s="11"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -1376,13 +1380,15 @@
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="12">
+        <v>2</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14"/>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="58"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="15" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1400,7 @@
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="61"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
@@ -1406,7 +1412,7 @@
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="69" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1417,10 +1423,12 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="58"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="6" t="s">
         <v>9</v>
       </c>
@@ -1429,10 +1437,12 @@
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="61"/>
+      <c r="A11" s="71"/>
       <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1444,7 +1454,7 @@
       <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="72" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1455,10 +1465,12 @@
       <c r="E12" s="12"/>
       <c r="F12" s="13"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="58"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="15" t="s">
         <v>8</v>
       </c>
@@ -1467,14 +1479,18 @@
       <c r="E13" s="15"/>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="15"/>
+      <c r="H13" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="61"/>
+      <c r="A14" s="71"/>
       <c r="B14" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="19">
+        <v>2</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="18"/>
       <c r="F14" s="19"/>
@@ -1482,7 +1498,7 @@
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="69" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1493,10 +1509,12 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="58"/>
+      <c r="A16" s="70"/>
       <c r="B16" s="6" t="s">
         <v>9</v>
       </c>
@@ -1508,19 +1526,21 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="61"/>
+      <c r="A17" s="71"/>
       <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="10">
+        <v>2</v>
+      </c>
       <c r="G17" s="11"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="72" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -1531,10 +1551,12 @@
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="12"/>
+      <c r="H18" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="58"/>
+      <c r="A19" s="70"/>
       <c r="B19" s="15" t="s">
         <v>8</v>
       </c>
@@ -1543,10 +1565,12 @@
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="15"/>
+      <c r="H19" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="61"/>
+      <c r="A20" s="71"/>
       <c r="B20" s="18" t="s">
         <v>10</v>
       </c>
@@ -1558,7 +1582,7 @@
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="69" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1566,29 +1590,35 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="5"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="58"/>
+      <c r="A22" s="70"/>
       <c r="B22" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>1</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
       <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="61"/>
+      <c r="A23" s="71"/>
       <c r="B23" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="10">
+        <v>2</v>
+      </c>
       <c r="D23" s="11"/>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
@@ -1596,7 +1626,7 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="72" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -1607,10 +1637,12 @@
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="58"/>
+      <c r="A25" s="70"/>
       <c r="B25" s="15" t="s">
         <v>8</v>
       </c>
@@ -1619,10 +1651,12 @@
       <c r="E25" s="15"/>
       <c r="F25" s="16"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="15"/>
+      <c r="H25" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="61"/>
+      <c r="A26" s="71"/>
       <c r="B26" s="18" t="s">
         <v>10</v>
       </c>
@@ -1631,10 +1665,12 @@
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
       <c r="G26" s="20"/>
-      <c r="H26" s="18"/>
+      <c r="H26" s="18">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1645,10 +1681,12 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="58"/>
+      <c r="A28" s="70"/>
       <c r="B28" s="6" t="s">
         <v>9</v>
       </c>
@@ -1657,10 +1695,12 @@
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="61"/>
+      <c r="A29" s="71"/>
       <c r="B29" s="9" t="s">
         <v>10</v>
       </c>
@@ -1669,10 +1709,12 @@
       <c r="E29" s="9"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="72" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -1680,80 +1722,86 @@
       </c>
       <c r="C30" s="22"/>
       <c r="D30" s="23"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="21">
+        <v>1</v>
+      </c>
       <c r="F30" s="22"/>
       <c r="G30" s="23"/>
       <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="58"/>
+      <c r="A31" s="70"/>
       <c r="B31" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="15">
+        <v>2</v>
+      </c>
       <c r="F31" s="16"/>
       <c r="G31" s="17"/>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="61"/>
+      <c r="A32" s="71"/>
       <c r="B32" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
-      <c r="E32" s="18"/>
+      <c r="E32" s="18">
+        <v>2</v>
+      </c>
       <c r="F32" s="19"/>
       <c r="G32" s="20"/>
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="67">
+      <c r="B33" s="58"/>
+      <c r="C33" s="63">
         <f>SUM(C3:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="68">
+        <v>4</v>
+      </c>
+      <c r="D33" s="65">
         <f>SUM(D3:D32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="75">
+      <c r="E33" s="61">
         <f>SUM(E3:E32)+C33+D33</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="67">
+        <v>14</v>
+      </c>
+      <c r="F33" s="63">
         <f>SUM(F3:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="68">
+        <v>4</v>
+      </c>
+      <c r="G33" s="65">
         <f>SUM(G3:G32)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="77">
+      <c r="H33" s="67">
         <f>SUM(H3:H32)+F33+G33</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="70"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="70"/>
-      <c r="N33" s="70"/>
+        <v>25</v>
+      </c>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
     </row>
     <row r="34" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="73"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="78"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="68"/>
       <c r="I34" s="56"/>
       <c r="J34" s="56"/>
       <c r="K34" s="56"/>
@@ -1763,6 +1811,21 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="K33:K34"/>
     <mergeCell ref="L33:L34"/>
     <mergeCell ref="M33:M34"/>
@@ -1774,21 +1837,6 @@
     <mergeCell ref="H33:H34"/>
     <mergeCell ref="I33:I34"/>
     <mergeCell ref="J33:J34"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -1800,7 +1848,7 @@
   <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1813,49 +1861,53 @@
       </c>
       <c r="C1" s="80"/>
       <c r="D1" s="80"/>
-      <c r="E1" s="72"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="82" t="str">
         <f>Category!F1</f>
         <v>Elky</v>
       </c>
       <c r="G1" s="80"/>
       <c r="H1" s="80"/>
-      <c r="I1" s="72"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="84"/>
-      <c r="B2" s="73"/>
+      <c r="B2" s="59"/>
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="73"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="59"/>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
-      <c r="I2" s="74"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="86"/>
+      <c r="B3" s="86">
+        <v>11</v>
+      </c>
       <c r="C3" s="80"/>
       <c r="D3" s="80"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="87"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="87">
+        <v>16</v>
+      </c>
       <c r="G3" s="80"/>
       <c r="H3" s="80"/>
-      <c r="I3" s="72"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="84"/>
-      <c r="B4" s="73"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="81"/>
       <c r="D4" s="81"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="73"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="59"/>
       <c r="G4" s="81"/>
       <c r="H4" s="81"/>
-      <c r="I4" s="74"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="44"/>
@@ -2108,26 +2160,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1"/>
-      <c r="C1" s="62" t="str">
+      <c r="C1" s="75" t="str">
         <f>Category!C1</f>
         <v>Southern Buckeye Regional Champions</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65" t="str">
+      <c r="D1" s="76"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="78" t="str">
         <f>Category!F1</f>
         <v>Elky</v>
       </c>
-      <c r="G1" s="63"/>
-      <c r="H1" s="64"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
@@ -2173,7 +2225,9 @@
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
       <c r="G3" s="5"/>
       <c r="H3" s="3"/>
     </row>
@@ -2182,7 +2236,9 @@
       <c r="B4" s="29">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7">
+        <v>2</v>
+      </c>
       <c r="D4" s="8"/>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
@@ -2194,7 +2250,9 @@
       <c r="B5" s="29">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7">
+        <v>3</v>
+      </c>
       <c r="D5" s="8"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
@@ -2206,7 +2264,9 @@
       <c r="B6" s="29">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
@@ -2221,7 +2281,9 @@
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="10"/>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
       <c r="G7" s="11"/>
       <c r="H7" s="9"/>
     </row>
@@ -2232,7 +2294,9 @@
       <c r="B8" s="31">
         <v>6</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
       <c r="D8" s="14"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
@@ -2244,7 +2308,9 @@
       <c r="B9" s="32">
         <v>7</v>
       </c>
-      <c r="C9" s="16"/>
+      <c r="C9" s="16">
+        <v>3</v>
+      </c>
       <c r="D9" s="17"/>
       <c r="E9" s="15"/>
       <c r="F9" s="16"/>
@@ -2268,7 +2334,9 @@
       <c r="B11" s="32">
         <v>9</v>
       </c>
-      <c r="C11" s="16"/>
+      <c r="C11" s="16">
+        <v>3</v>
+      </c>
       <c r="D11" s="17"/>
       <c r="E11" s="15"/>
       <c r="F11" s="16"/>
@@ -2280,7 +2348,9 @@
       <c r="B12" s="33">
         <v>10</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="19">
+        <v>2</v>
+      </c>
       <c r="D12" s="20"/>
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
@@ -2298,7 +2368,9 @@
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
@@ -2310,7 +2382,9 @@
       <c r="D14" s="8"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8">
+        <v>2</v>
+      </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2360,7 +2434,9 @@
       <c r="D18" s="14"/>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="14">
+        <v>2</v>
+      </c>
       <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
@@ -2372,7 +2448,9 @@
       <c r="D19" s="17"/>
       <c r="E19" s="15"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17">
+        <v>2</v>
+      </c>
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
@@ -2396,7 +2474,9 @@
       <c r="D21" s="17"/>
       <c r="E21" s="15"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17">
+        <v>3</v>
+      </c>
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2404,7 +2484,9 @@
       <c r="B22" s="33">
         <v>20</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="19">
+        <v>2</v>
+      </c>
       <c r="D22" s="20"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19"/>
@@ -2433,7 +2515,9 @@
       <c r="C24" s="7"/>
       <c r="D24" s="8"/>
       <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
       <c r="G24" s="8"/>
       <c r="H24" s="6"/>
     </row>
@@ -2458,7 +2542,9 @@
       <c r="D26" s="8"/>
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="8">
+        <v>2</v>
+      </c>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2470,7 +2556,9 @@
       <c r="D27" s="11"/>
       <c r="E27" s="9"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
+      <c r="G27" s="11">
+        <v>2</v>
+      </c>
       <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
@@ -2483,7 +2571,9 @@
       <c r="C28" s="22"/>
       <c r="D28" s="23"/>
       <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
+      <c r="F28" s="22">
+        <v>2</v>
+      </c>
       <c r="G28" s="23"/>
       <c r="H28" s="21"/>
     </row>
@@ -2495,7 +2585,9 @@
       <c r="C29" s="16"/>
       <c r="D29" s="17"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="16"/>
+      <c r="F29" s="16">
+        <v>2</v>
+      </c>
       <c r="G29" s="17"/>
       <c r="H29" s="15"/>
     </row>
@@ -2507,7 +2599,9 @@
       <c r="C30" s="16"/>
       <c r="D30" s="17"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="16"/>
+      <c r="F30" s="16">
+        <v>2</v>
+      </c>
       <c r="G30" s="17"/>
       <c r="H30" s="15"/>
     </row>
@@ -2519,7 +2613,9 @@
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="16"/>
+      <c r="F31" s="16">
+        <v>2</v>
+      </c>
       <c r="G31" s="17"/>
       <c r="H31" s="15"/>
     </row>
@@ -2528,7 +2624,9 @@
       <c r="B32" s="33">
         <v>30</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="19">
+        <v>2</v>
+      </c>
       <c r="D32" s="20"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19"/>
@@ -2536,33 +2634,33 @@
       <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="67">
+      <c r="B33" s="58"/>
+      <c r="C33" s="63">
         <f>SUM(C3:C32)</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="68">
+        <v>23</v>
+      </c>
+      <c r="D33" s="65">
         <f>SUM(D3:D32)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="77">
+      <c r="E33" s="67">
         <f>SUM(E3:E32)+C33+D33</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="67">
+        <v>23</v>
+      </c>
+      <c r="F33" s="63">
         <f>SUM(F3:F32)</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="68">
+        <v>14</v>
+      </c>
+      <c r="G33" s="65">
         <f>SUM(G3:G32)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H33" s="88">
         <f>SUM(H3:H32)+F33+G33</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I33" s="44"/>
       <c r="J33" s="44"/>
@@ -2572,14 +2670,14 @@
       <c r="N33" s="44"/>
     </row>
     <row r="34" spans="1:14" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="73"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="78"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="68"/>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
       <c r="K34" s="44"/>
@@ -2613,192 +2711,197 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="55"/>
+      <c r="A1" s="73"/>
       <c r="B1" s="56"/>
-      <c r="C1" s="93" t="str">
+      <c r="C1" s="95" t="str">
         <f>Category!C1</f>
         <v>Southern Buckeye Regional Champions</v>
       </c>
       <c r="D1" s="80"/>
       <c r="E1" s="80"/>
       <c r="F1" s="80"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="94" t="str">
+      <c r="G1" s="58"/>
+      <c r="H1" s="96" t="str">
         <f>Category!F1</f>
         <v>Elky</v>
       </c>
       <c r="I1" s="80"/>
       <c r="J1" s="80"/>
       <c r="K1" s="80"/>
-      <c r="L1" s="72"/>
+      <c r="L1" s="58"/>
     </row>
     <row r="2" spans="1:12" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
-      <c r="C2" s="73"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="81"/>
       <c r="E2" s="81"/>
       <c r="F2" s="81"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="73"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="81"/>
       <c r="J2" s="81"/>
       <c r="K2" s="81"/>
-      <c r="L2" s="74"/>
+      <c r="L2" s="60"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="95">
+      <c r="B3" s="58"/>
+      <c r="C3" s="93">
         <f>Category!E33</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="80"/>
       <c r="F3" s="80"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="95">
+      <c r="G3" s="58"/>
+      <c r="H3" s="93">
         <f>Category!H33</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I3" s="80"/>
       <c r="J3" s="80"/>
       <c r="K3" s="80"/>
-      <c r="L3" s="72"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="73"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="73"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="81"/>
       <c r="E4" s="81"/>
       <c r="F4" s="81"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="73"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="59"/>
       <c r="I4" s="81"/>
       <c r="J4" s="81"/>
       <c r="K4" s="81"/>
-      <c r="L4" s="74"/>
+      <c r="L4" s="60"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="96">
+      <c r="B5" s="58"/>
+      <c r="C5" s="94">
         <f>Alphabet!B3</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D5" s="80"/>
       <c r="E5" s="80"/>
       <c r="F5" s="80"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="96">
+      <c r="G5" s="58"/>
+      <c r="H5" s="94">
         <f>Alphabet!F3</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I5" s="80"/>
       <c r="J5" s="80"/>
       <c r="K5" s="80"/>
-      <c r="L5" s="72"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:12" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="73"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="73"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="81"/>
       <c r="E6" s="81"/>
       <c r="F6" s="81"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="73"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="81"/>
       <c r="J6" s="81"/>
       <c r="K6" s="81"/>
-      <c r="L6" s="74"/>
+      <c r="L6" s="60"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A7" s="95" t="s">
+      <c r="A7" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="95">
+      <c r="B7" s="58"/>
+      <c r="C7" s="93">
         <f>Lightning!E33</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D7" s="80"/>
       <c r="E7" s="80"/>
       <c r="F7" s="80"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="95">
+      <c r="G7" s="58"/>
+      <c r="H7" s="93">
         <f>Lightning!H33</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I7" s="80"/>
       <c r="J7" s="80"/>
       <c r="K7" s="80"/>
-      <c r="L7" s="72"/>
+      <c r="L7" s="58"/>
     </row>
     <row r="8" spans="1:12" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="73"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="81"/>
       <c r="E8" s="81"/>
       <c r="F8" s="81"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="73"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="59"/>
       <c r="I8" s="81"/>
       <c r="J8" s="81"/>
       <c r="K8" s="81"/>
-      <c r="L8" s="74"/>
+      <c r="L8" s="60"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="72"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="79">
         <f>SUM(C3:G8)</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D9" s="80"/>
       <c r="E9" s="80"/>
       <c r="F9" s="80"/>
-      <c r="G9" s="72"/>
+      <c r="G9" s="58"/>
       <c r="H9" s="82">
         <f>SUM(H3:L8)</f>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="I9" s="80"/>
       <c r="J9" s="80"/>
       <c r="K9" s="80"/>
-      <c r="L9" s="72"/>
+      <c r="L9" s="58"/>
     </row>
     <row r="10" spans="1:12" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="73"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="73"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="81"/>
       <c r="E10" s="81"/>
       <c r="F10" s="81"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="73"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="59"/>
       <c r="I10" s="81"/>
       <c r="J10" s="81"/>
       <c r="K10" s="81"/>
-      <c r="L10" s="74"/>
+      <c r="L10" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:G2"/>
+    <mergeCell ref="H1:L2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:G4"/>
     <mergeCell ref="A9:B10"/>
     <mergeCell ref="C9:G10"/>
     <mergeCell ref="H9:L10"/>
@@ -2809,11 +2912,6 @@
     <mergeCell ref="C7:G8"/>
     <mergeCell ref="H7:L8"/>
     <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:G2"/>
-    <mergeCell ref="H1:L2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2854,15 +2952,15 @@
       </c>
       <c r="B2" s="35">
         <f>3*C2+2*D2</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C2" s="48">
         <f>COUNTIF(Category!C3:C32, "&gt;2")+COUNTIF(Lightning!C3:C32, "&gt;2")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2" s="38">
         <f>COUNTIFS(Category!C3:C32, "&gt;0",Category!C3:C32, "&lt;3" )+COUNTIFS(Lightning!C3:C32, "&gt;0",Lightning!C3:C32, "&lt;3" )</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -2890,7 +2988,7 @@
       </c>
       <c r="B4" s="36">
         <f>3*C4+2*D4</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C4" s="50">
         <f>COUNTIF(Category!F3:F32, "&gt;2")+COUNTIF(Lightning!F3:F32, "&gt;2")</f>
@@ -2898,7 +2996,7 @@
       </c>
       <c r="D4" s="39">
         <f>COUNTIFS(Category!F3:F32, "&gt;0",Category!F3:F32, "&lt;3" )+COUNTIFS(Lightning!F3:F32, "&gt;0",Lightning!F3:F32, "&lt;3" )</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -2908,15 +3006,15 @@
       </c>
       <c r="B5" s="37">
         <f>3*C5+2*D5</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C5" s="51">
         <f>COUNTIF(Category!G3:G32,"&gt;2")+COUNTIF(Lightning!G3:G32,"&gt;2")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="40">
         <f>COUNTIFS(Category!G3:G32, "&gt;0",Category!G3:G32, "&lt;3" )+COUNTIFS(Lightning!G3:G32, "&gt;0",Lightning!G3:G32, "&lt;3" )</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2928,8 +3026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="29.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2954,46 +3052,46 @@
         <v>Will Reuter</v>
       </c>
       <c r="B2" s="35">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C2" s="48">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D2" s="38">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="46">
-        <v>0</v>
+      <c r="A3" s="46" t="str">
+        <v>Abigail Friedstrom</v>
       </c>
       <c r="B3" s="36">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C3" s="49">
         <v>0</v>
       </c>
       <c r="D3" s="39">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="46" t="str">
-        <v>Abigail Friedstrom</v>
+        <v>Ky Reckamp</v>
       </c>
       <c r="B4" s="36">
+        <v>15</v>
+      </c>
+      <c r="C4" s="50">
+        <v>1</v>
+      </c>
+      <c r="D4" s="39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="47">
         <v>0</v>
-      </c>
-      <c r="C4" s="50">
-        <v>0</v>
-      </c>
-      <c r="D4" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="29.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="47" t="str">
-        <v>Ky Reckamp</v>
       </c>
       <c r="B5" s="37">
         <v>0</v>

</xml_diff>